<commit_message>
Penyelesaian CRUD pelanggan, pengguna, jenis program dan program
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>no</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>laporan jadwal keberangkatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">persyaratan haji dan umroh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rukun haji dan umroh </t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E20"/>
+  <dimension ref="B3:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,29 +529,26 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -553,10 +556,13 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -564,7 +570,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -575,7 +581,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -586,7 +592,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -597,33 +603,55 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>